<commit_message>
added PLS and example for loading Excel sheets
</commit_message>
<xml_diff>
--- a/data/Pivot and Unpivot Data.xlsx
+++ b/data/Pivot and Unpivot Data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\np-spotfire\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4787DC3-AF2F-4D2C-BFB1-176FA21ED27F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ABBFA18-7091-45FE-A44C-30BB5E172C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{D033B4F3-C812-4D1A-B237-CA9BD69AB7C4}"/>
+    <workbookView xWindow="15890" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{D033B4F3-C812-4D1A-B237-CA9BD69AB7C4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Long table" sheetId="1" r:id="rId1"/>
+    <sheet name="Wide table" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="21">
   <si>
     <t>ExperimentId</t>
   </si>
@@ -63,6 +64,42 @@
   </si>
   <si>
     <t>Cost</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>Jan</t>
+  </si>
+  <si>
+    <t>Feb</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>OrderId</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Test4</t>
+  </si>
+  <si>
+    <t>Test5</t>
+  </si>
+  <si>
+    <t>Test6</t>
   </si>
 </sst>
 </file>
@@ -115,6 +152,35 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EEC243F8-4BA3-47F2-9DA0-E8336B71B343}" name="Table1" displayName="Table1" ref="A1:D7" totalsRowShown="0">
+  <autoFilter ref="A1:D7" xr:uid="{EEC243F8-4BA3-47F2-9DA0-E8336B71B343}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{FA4DED9A-CF5A-42CD-88E3-C47EEB0A0404}" name="ExperimentId"/>
+    <tableColumn id="2" xr3:uid="{B1FAD3D8-1FAD-4CEE-80CB-2FAE72E2922F}" name="Test"/>
+    <tableColumn id="3" xr3:uid="{A26384AC-58DF-4C50-859C-218D82CFF25E}" name="Outcome"/>
+    <tableColumn id="4" xr3:uid="{DA4B3131-D313-4D6E-A22D-FF8D18BFFA17}" name="Cost"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CAF4C19D-1D56-4405-9D18-055E73945DA2}" name="Table2" displayName="Table2" ref="A1:G5" totalsRowShown="0">
+  <autoFilter ref="A1:G5" xr:uid="{CAF4C19D-1D56-4405-9D18-055E73945DA2}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{36711792-29F3-4A8D-B06B-67A1155FFB08}" name="ExperimentId"/>
+    <tableColumn id="2" xr3:uid="{35CB5132-60B8-4896-8136-6FD9E0F94E66}" name="Test1"/>
+    <tableColumn id="3" xr3:uid="{E3B852F4-3041-4D9B-A5DE-7C28D0412642}" name="Test2"/>
+    <tableColumn id="4" xr3:uid="{A8562A7C-EBC1-4333-8C0B-7D4D5989AC1E}" name="Test3"/>
+    <tableColumn id="5" xr3:uid="{92CF28EC-8012-4E1D-B008-81BCA3832537}" name="Test4"/>
+    <tableColumn id="6" xr3:uid="{B1866FBE-48FF-4183-A41F-92E68782219F}" name="Test5"/>
+    <tableColumn id="7" xr3:uid="{E76880CC-F7A4-49B2-B0C6-BB42D0F86F87}" name="Test6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -414,22 +480,193 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83BD9BC5-BFA6-4028-A083-F3D3AF054F26}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+      <c r="H3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>150</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>320</v>
+      </c>
+      <c r="G5">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7">
+        <v>40</v>
+      </c>
+      <c r="H7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E098781F-1C90-488B-A486-D3245E730B24}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -438,8 +675,17 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -452,8 +698,17 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -466,8 +721,17 @@
       <c r="D3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -480,8 +744,17 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -494,106 +767,20 @@
       <c r="D5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>5</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D12">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>6</v>
-      </c>
-      <c r="B13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>6</v>
-      </c>
-      <c r="B14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15">
-        <v>40</v>
+      <c r="E5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>